<commit_message>
filled out grid, finished input.txt & ignore empty lines
</commit_message>
<xml_diff>
--- a/MaxwellMichael-grid.xlsx
+++ b/MaxwellMichael-grid.xlsx
@@ -1,16 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PROLE\Documents\GitHub\poker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F66AA71-683E-4E96-83D7-0E3B09EB4E11}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="179021" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="126">
-  <si>
-    <t>yes/no</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="214">
   <si>
     <t>You have coded your dependencies using Maven</t>
   </si>
@@ -464,12 +472,279 @@
   <si>
     <t>This assignment is worth 20% of your final grade. A2 and  A3 will be worth 15% each.</t>
   </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Maxwell</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>testRoyalFlush</t>
+  </si>
+  <si>
+    <t>testStraightFlush</t>
+  </si>
+  <si>
+    <t>testFullHouse</t>
+  </si>
+  <si>
+    <t>testTwoPairs</t>
+  </si>
+  <si>
+    <t>testFourOfKind</t>
+  </si>
+  <si>
+    <t>testFlush</t>
+  </si>
+  <si>
+    <t>testStraight</t>
+  </si>
+  <si>
+    <t>testSet</t>
+  </si>
+  <si>
+    <t>testSinglePair</t>
+  </si>
+  <si>
+    <t>test1AwayFlush</t>
+  </si>
+  <si>
+    <t>test2AwayFlush</t>
+  </si>
+  <si>
+    <t>test1AwayStraightFlush</t>
+  </si>
+  <si>
+    <t>test1AwayRoyalFlush</t>
+  </si>
+  <si>
+    <t>test1AwayStraight</t>
+  </si>
+  <si>
+    <t>test3CardSequence</t>
+  </si>
+  <si>
+    <t>testComparingDifferentHands</t>
+  </si>
+  <si>
+    <t>testNoExchange</t>
+  </si>
+  <si>
+    <t>test1AwayRoyalFlushExchange</t>
+  </si>
+  <si>
+    <t>test1AwayStraightFlushExchange</t>
+  </si>
+  <si>
+    <t>test1AwayFourOfKind</t>
+  </si>
+  <si>
+    <t>testIndependentOfExchange</t>
+  </si>
+  <si>
+    <t>test1AwayFlushExchange</t>
+  </si>
+  <si>
+    <t>test1AwayStraightExchange</t>
+  </si>
+  <si>
+    <t>test2AwayFlushExchange</t>
+  </si>
+  <si>
+    <t>test1AwayFourOfKindExchange</t>
+  </si>
+  <si>
+    <t>test3CardSequenceExchange</t>
+  </si>
+  <si>
+    <t>testTwoPairExchange</t>
+  </si>
+  <si>
+    <t>testSinglePairExchange</t>
+  </si>
+  <si>
+    <t>testNothingHandExchange</t>
+  </si>
+  <si>
+    <t>testCompareRoyalFlushes</t>
+  </si>
+  <si>
+    <t>testCompareStraightFlushes</t>
+  </si>
+  <si>
+    <t>testCompareFourOfAKinds</t>
+  </si>
+  <si>
+    <t>testCompareFullHouses</t>
+  </si>
+  <si>
+    <t>testCompareThreeOfAKinds</t>
+  </si>
+  <si>
+    <t>testCompareStraights</t>
+  </si>
+  <si>
+    <t>testCompareTwoPairs</t>
+  </si>
+  <si>
+    <t>testCompareSinglePairs</t>
+  </si>
+  <si>
+    <t>testCompareHighCards</t>
+  </si>
+  <si>
+    <t>testCompareFlushes</t>
+  </si>
+  <si>
+    <t>bonus1.txt</t>
+  </si>
+  <si>
+    <t>bonus2.txt</t>
+  </si>
+  <si>
+    <t>input.txt 3</t>
+  </si>
+  <si>
+    <t>input.txt 4</t>
+  </si>
+  <si>
+    <t>input.txt 5</t>
+  </si>
+  <si>
+    <t>input.txt 6</t>
+  </si>
+  <si>
+    <t>input.txt 7</t>
+  </si>
+  <si>
+    <t>input.txt 8</t>
+  </si>
+  <si>
+    <t>input.txt 9</t>
+  </si>
+  <si>
+    <t>input.txt 10</t>
+  </si>
+  <si>
+    <t>input.txt 11</t>
+  </si>
+  <si>
+    <t>input.txt 12</t>
+  </si>
+  <si>
+    <t>input.txt 13</t>
+  </si>
+  <si>
+    <t>input.txt 14</t>
+  </si>
+  <si>
+    <t>input.txt 15</t>
+  </si>
+  <si>
+    <t>input.txt 16</t>
+  </si>
+  <si>
+    <t>input.txt 17</t>
+  </si>
+  <si>
+    <t>input.txt 18</t>
+  </si>
+  <si>
+    <t>input.txt 19</t>
+  </si>
+  <si>
+    <t>input.txt 20</t>
+  </si>
+  <si>
+    <t>input.txt 21</t>
+  </si>
+  <si>
+    <t>input.txt 22</t>
+  </si>
+  <si>
+    <t>input.txt 23</t>
+  </si>
+  <si>
+    <t>input.txt 24</t>
+  </si>
+  <si>
+    <t>input.txt 25</t>
+  </si>
+  <si>
+    <t>input.txt 26</t>
+  </si>
+  <si>
+    <t>input.txt 27</t>
+  </si>
+  <si>
+    <t>input.txt 29</t>
+  </si>
+  <si>
+    <t>input.txt 30</t>
+  </si>
+  <si>
+    <t>input.txt 31</t>
+  </si>
+  <si>
+    <t>input.txt 32</t>
+  </si>
+  <si>
+    <t>input.txt 33</t>
+  </si>
+  <si>
+    <t>input.txt 34</t>
+  </si>
+  <si>
+    <t>input.txt 35</t>
+  </si>
+  <si>
+    <t>input.txt 36</t>
+  </si>
+  <si>
+    <t>input.txt 37</t>
+  </si>
+  <si>
+    <t>input.txt 38</t>
+  </si>
+  <si>
+    <t>input.txt 39</t>
+  </si>
+  <si>
+    <t>input.txt 40</t>
+  </si>
+  <si>
+    <t>input.txt 41</t>
+  </si>
+  <si>
+    <t>input.txt 42</t>
+  </si>
+  <si>
+    <t>input.txt 43</t>
+  </si>
+  <si>
+    <t>input.txt 44</t>
+  </si>
+  <si>
+    <t>input.txt 45</t>
+  </si>
+  <si>
+    <t>input.txt 46</t>
+  </si>
+  <si>
+    <t>input.txt 47</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -535,8 +810,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -573,8 +862,18 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -582,8 +881,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="221">
+  <cellStyleXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -805,8 +1119,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -828,8 +1144,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="222" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="221"/>
   </cellXfs>
-  <cellStyles count="221">
+  <cellStyles count="223">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -940,6 +1258,7 @@
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="221" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1051,9 +1370,18 @@
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="222" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1378,163 +1706,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="85.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="85.625" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="4"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="G1" s="2">
+        <v>101006277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1542,18 +1879,20 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14">
         <v>1</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1561,18 +1900,20 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1580,18 +1921,20 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16">
         <v>1</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1599,18 +1942,20 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1618,18 +1963,20 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1637,18 +1984,20 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19">
         <v>1</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1656,18 +2005,20 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1675,18 +2026,20 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1694,18 +2047,20 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22">
         <v>2</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1713,24 +2068,26 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C23"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24">
         <v>5</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1738,24 +2095,26 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C25"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26">
         <v>1</v>
       </c>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -1763,18 +2122,20 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27">
         <v>1</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -1782,18 +2143,20 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28">
         <v>1</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1801,18 +2164,20 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -1820,18 +2185,20 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30">
         <v>1</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -1839,18 +2206,20 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1858,18 +2227,20 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1877,18 +2248,20 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -1896,18 +2269,20 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34">
         <v>1</v>
       </c>
-      <c r="E34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -1915,21 +2290,21 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C35"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C37" s="6"/>
       <c r="D37">
@@ -1937,57 +2312,57 @@
       </c>
       <c r="M37" s="4"/>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C38" s="6"/>
       <c r="D38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C39" s="6"/>
       <c r="D39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40">
         <v>0.5</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C41"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42"/>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C43" s="8">
         <f>SUM(J45:J101)</f>
@@ -1998,371 +2373,439 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E44" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45">
         <v>0.5</v>
       </c>
-      <c r="E45" s="2"/>
+      <c r="E45" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
+      <c r="H45" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="I45" s="2"/>
       <c r="J45" s="6"/>
       <c r="K45">
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46">
         <v>0.5</v>
       </c>
-      <c r="E46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
+      <c r="H46" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="I46" s="2"/>
       <c r="J46" s="6"/>
       <c r="K46">
         <v>0.5</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47">
         <v>0.5</v>
       </c>
-      <c r="E47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
+      <c r="H47" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="I47" s="2"/>
       <c r="J47" s="6"/>
       <c r="K47">
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48">
         <v>0.5</v>
       </c>
-      <c r="E48" s="2"/>
+      <c r="E48" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
+      <c r="H48" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="I48" s="2"/>
       <c r="J48" s="6"/>
       <c r="K48">
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49">
         <v>0.5</v>
       </c>
-      <c r="E49" s="2"/>
+      <c r="E49" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
+      <c r="H49" s="2" t="s">
+        <v>174</v>
+      </c>
       <c r="I49" s="2"/>
       <c r="J49" s="6"/>
       <c r="K49">
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50">
         <v>0.5</v>
       </c>
-      <c r="E50" s="2"/>
+      <c r="E50" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
+      <c r="H50" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="I50" s="2"/>
       <c r="J50" s="6"/>
       <c r="K50">
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51">
         <v>0.5</v>
       </c>
-      <c r="E51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
+      <c r="H51" s="2" t="s">
+        <v>176</v>
+      </c>
       <c r="I51" s="2"/>
       <c r="J51" s="6"/>
       <c r="K51">
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52">
         <v>0.5</v>
       </c>
-      <c r="E52" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
+      <c r="H52" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="I52" s="2"/>
       <c r="J52" s="6"/>
       <c r="K52">
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53">
         <v>0.5</v>
       </c>
-      <c r="E53" s="2"/>
+      <c r="E53" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
+      <c r="H53" s="2" t="s">
+        <v>178</v>
+      </c>
       <c r="I53" s="2"/>
       <c r="J53" s="6"/>
       <c r="K53">
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54">
         <v>0.5</v>
       </c>
-      <c r="E54" s="2"/>
+      <c r="E54" s="2" t="s">
+        <v>151</v>
+      </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
+      <c r="H54" s="2" t="s">
+        <v>179</v>
+      </c>
       <c r="I54" s="2"/>
       <c r="J54" s="6"/>
       <c r="K54">
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55">
         <v>0.5</v>
       </c>
-      <c r="E55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
+      <c r="H55" s="2" t="s">
+        <v>180</v>
+      </c>
       <c r="I55" s="2"/>
       <c r="J55" s="6"/>
       <c r="K55">
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56">
         <v>0.5</v>
       </c>
-      <c r="E56" s="2"/>
+      <c r="E56" s="2" t="s">
+        <v>153</v>
+      </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
+      <c r="H56" s="2" t="s">
+        <v>181</v>
+      </c>
       <c r="I56" s="2"/>
       <c r="J56" s="6"/>
       <c r="K56">
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57">
         <v>0.5</v>
       </c>
-      <c r="E57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
+      <c r="H57" s="2" t="s">
+        <v>182</v>
+      </c>
       <c r="I57" s="2"/>
       <c r="J57" s="6"/>
       <c r="K57">
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C58" s="6"/>
       <c r="D58">
         <v>0.5</v>
       </c>
-      <c r="E58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
+      <c r="H58" s="2" t="s">
+        <v>183</v>
+      </c>
       <c r="I58" s="2"/>
       <c r="J58" s="6"/>
       <c r="K58">
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59">
         <v>0.5</v>
       </c>
-      <c r="E59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>156</v>
+      </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
+      <c r="H59" s="2" t="s">
+        <v>184</v>
+      </c>
       <c r="I59" s="2"/>
       <c r="J59" s="6"/>
       <c r="K59">
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60">
         <v>0.5</v>
       </c>
-      <c r="E60" s="2"/>
+      <c r="E60" s="2" t="s">
+        <v>157</v>
+      </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
+      <c r="H60" s="2" t="s">
+        <v>185</v>
+      </c>
       <c r="I60" s="2"/>
       <c r="J60" s="6"/>
       <c r="K60">
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C61"/>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C62"/>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C63" s="6"/>
       <c r="D63">
         <v>0.25</v>
       </c>
-      <c r="E63" s="2"/>
+      <c r="E63" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
+      <c r="H63" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="I63" s="2"/>
       <c r="J63" s="6"/>
       <c r="K63">
@@ -2370,21 +2813,25 @@
       </c>
       <c r="M63" s="9"/>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C64" s="6"/>
       <c r="D64">
         <v>0.5</v>
       </c>
-      <c r="E64" s="2"/>
+      <c r="E64" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
+      <c r="H64" s="2" t="s">
+        <v>187</v>
+      </c>
       <c r="I64" s="2"/>
       <c r="J64" s="6"/>
       <c r="K64">
@@ -2392,21 +2839,25 @@
       </c>
       <c r="M64" s="9"/>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C65" s="6"/>
       <c r="D65">
         <v>0.25</v>
       </c>
-      <c r="E65" s="2"/>
+      <c r="E65" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
+      <c r="H65" s="2" t="s">
+        <v>188</v>
+      </c>
       <c r="I65" s="2"/>
       <c r="J65" s="6"/>
       <c r="K65">
@@ -2414,21 +2865,25 @@
       </c>
       <c r="M65" s="9"/>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66">
         <v>0.25</v>
       </c>
-      <c r="E66" s="2"/>
+      <c r="E66" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
+      <c r="H66" s="2" t="s">
+        <v>189</v>
+      </c>
       <c r="I66" s="2"/>
       <c r="J66" s="6"/>
       <c r="K66">
@@ -2436,21 +2891,25 @@
       </c>
       <c r="M66" s="9"/>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67">
         <v>0.25</v>
       </c>
-      <c r="E67" s="2"/>
+      <c r="E67" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
+      <c r="H67" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="I67" s="2"/>
       <c r="J67" s="6"/>
       <c r="K67">
@@ -2458,21 +2917,25 @@
       </c>
       <c r="M67" s="9"/>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68">
         <v>0.25</v>
       </c>
-      <c r="E68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
+      <c r="H68" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="I68" s="2"/>
       <c r="J68" s="6"/>
       <c r="K68">
@@ -2480,21 +2943,25 @@
       </c>
       <c r="M68" s="9"/>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69">
         <v>0.25</v>
       </c>
-      <c r="E69" s="2"/>
+      <c r="E69" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
+      <c r="H69" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="I69" s="2"/>
       <c r="J69" s="6"/>
       <c r="K69">
@@ -2502,21 +2969,25 @@
       </c>
       <c r="M69" s="9"/>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C70" s="6"/>
       <c r="D70">
         <v>0.25</v>
       </c>
-      <c r="E70" s="2"/>
+      <c r="E70" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
+      <c r="H70" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="I70" s="2"/>
       <c r="J70" s="6"/>
       <c r="K70">
@@ -2524,21 +2995,25 @@
       </c>
       <c r="M70" s="9"/>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71">
         <v>0.25</v>
       </c>
-      <c r="E71" s="2"/>
+      <c r="E71" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
+      <c r="H71" s="2" t="s">
+        <v>194</v>
+      </c>
       <c r="I71" s="2"/>
       <c r="J71" s="6"/>
       <c r="K71">
@@ -2546,198 +3021,230 @@
       </c>
       <c r="M71" s="9"/>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C72"/>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C73"/>
       <c r="M73" s="9"/>
     </row>
-    <row r="74" spans="1:13" s="1" customFormat="1">
+    <row r="74" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="75" spans="1:13">
-      <c r="A75" t="s">
-        <v>18</v>
-      </c>
       <c r="B75" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75">
         <v>0.5</v>
       </c>
-      <c r="E75" s="2"/>
+      <c r="E75" s="2" t="s">
+        <v>158</v>
+      </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
+      <c r="H75" s="2" t="s">
+        <v>195</v>
+      </c>
       <c r="I75" s="2"/>
       <c r="J75" s="6"/>
       <c r="K75">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C76" s="6"/>
       <c r="D76">
         <v>0.5</v>
       </c>
-      <c r="E76" s="2"/>
+      <c r="E76" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
+      <c r="H76" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="I76" s="2"/>
       <c r="J76" s="6"/>
       <c r="K76">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C77" s="6"/>
       <c r="D77">
         <v>0.5</v>
       </c>
-      <c r="E77" s="2"/>
+      <c r="E77" s="2" t="s">
+        <v>159</v>
+      </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
+      <c r="H77" s="2" t="s">
+        <v>197</v>
+      </c>
       <c r="I77" s="2"/>
       <c r="J77" s="6"/>
       <c r="K77">
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78">
         <v>0.5</v>
       </c>
-      <c r="E78" s="2"/>
+      <c r="E78" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
+      <c r="H78" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="I78" s="2"/>
       <c r="J78" s="6"/>
       <c r="K78">
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C79" s="6"/>
       <c r="D79">
         <v>0.5</v>
       </c>
-      <c r="E79" s="2"/>
+      <c r="E79" s="2" t="s">
+        <v>161</v>
+      </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
+      <c r="H79" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="I79" s="2"/>
       <c r="J79" s="6"/>
       <c r="K79">
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80">
         <v>0.5</v>
       </c>
-      <c r="E80" s="2"/>
+      <c r="E80" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
+      <c r="H80" s="2" t="s">
+        <v>200</v>
+      </c>
       <c r="I80" s="2"/>
       <c r="J80" s="6"/>
       <c r="K80">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>25</v>
+      </c>
+      <c r="C81"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>26</v>
       </c>
-      <c r="C81"/>
-    </row>
-    <row r="82" spans="1:11">
-      <c r="A82" t="s">
-        <v>27</v>
-      </c>
       <c r="B82" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C82" s="6"/>
       <c r="D82">
         <v>0.5</v>
       </c>
-      <c r="E82" s="2"/>
+      <c r="E82" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
+      <c r="H82" s="2" t="s">
+        <v>201</v>
+      </c>
       <c r="I82" s="2"/>
       <c r="J82" s="6"/>
       <c r="K82">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C83" s="6"/>
       <c r="D83">
         <v>0.5</v>
       </c>
-      <c r="E83" s="2"/>
+      <c r="E83" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
+      <c r="H83" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="I83" s="2"/>
       <c r="J83" s="6"/>
       <c r="K83">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B84" s="4"/>
       <c r="D84" s="4"/>
@@ -2747,229 +3254,278 @@
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C85" s="6"/>
       <c r="D85">
         <v>0.5</v>
       </c>
-      <c r="E85" s="2"/>
+      <c r="E85" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
+      <c r="H85" s="2" t="s">
+        <v>203</v>
+      </c>
       <c r="I85" s="2"/>
       <c r="J85" s="6"/>
       <c r="K85">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C86" s="6"/>
       <c r="D86">
         <v>0.5</v>
       </c>
-      <c r="E86" s="2"/>
+      <c r="E86" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
+      <c r="H86" s="2" t="s">
+        <v>204</v>
+      </c>
       <c r="I86" s="2"/>
       <c r="J86" s="6"/>
       <c r="K86">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>31</v>
+      </c>
+      <c r="B87" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E87" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="F87" s="17"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I87" s="17"/>
+      <c r="J87" s="18"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="88" spans="1:11">
-      <c r="A88" t="s">
+      <c r="C88"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>33</v>
       </c>
-      <c r="C88"/>
-    </row>
-    <row r="89" spans="1:11">
-      <c r="A89" t="s">
-        <v>34</v>
-      </c>
       <c r="B89" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C89" s="6"/>
       <c r="D89">
         <v>0.5</v>
       </c>
-      <c r="E89" s="2"/>
+      <c r="E89" s="2" t="s">
+        <v>165</v>
+      </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
+      <c r="H89" s="2" t="s">
+        <v>206</v>
+      </c>
       <c r="I89" s="2"/>
       <c r="J89" s="6"/>
       <c r="K89">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="91" spans="1:11">
-      <c r="A91" t="s">
-        <v>36</v>
-      </c>
       <c r="B91" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C91" s="6"/>
       <c r="D91">
         <v>0.5</v>
       </c>
-      <c r="E91" s="2"/>
+      <c r="E91" s="2" t="s">
+        <v>166</v>
+      </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
+      <c r="H91" s="2" t="s">
+        <v>207</v>
+      </c>
       <c r="I91" s="2"/>
       <c r="J91" s="6"/>
       <c r="K91">
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="93" spans="1:11">
-      <c r="A93" t="s">
-        <v>38</v>
-      </c>
       <c r="B93" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C93" s="6"/>
       <c r="D93">
         <v>0.5</v>
       </c>
-      <c r="E93" s="2"/>
+      <c r="E93" s="2" t="s">
+        <v>166</v>
+      </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
+      <c r="H93" s="2" t="s">
+        <v>208</v>
+      </c>
       <c r="I93" s="2"/>
       <c r="J93" s="6"/>
       <c r="K93">
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C94" s="6"/>
       <c r="D94">
         <v>0.5</v>
       </c>
-      <c r="E94" s="2"/>
+      <c r="E94" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
+      <c r="H94" s="2" t="s">
+        <v>209</v>
+      </c>
       <c r="I94" s="2"/>
       <c r="J94" s="6"/>
       <c r="K94">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C95" s="6"/>
       <c r="D95">
         <v>0.5</v>
       </c>
-      <c r="E95" s="2"/>
+      <c r="E95" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
+      <c r="H95" s="2" t="s">
+        <v>210</v>
+      </c>
       <c r="I95" s="2"/>
       <c r="J95" s="6"/>
       <c r="K95">
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="97" spans="1:13">
-      <c r="A97" t="s">
-        <v>43</v>
-      </c>
       <c r="B97" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C97" s="6"/>
       <c r="D97">
         <v>0.5</v>
       </c>
-      <c r="E97" s="2"/>
+      <c r="E97" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
+      <c r="H97" s="2" t="s">
+        <v>211</v>
+      </c>
       <c r="I97" s="2"/>
       <c r="J97" s="6"/>
       <c r="K97">
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="99" spans="1:13">
-      <c r="A99" t="s">
-        <v>45</v>
-      </c>
       <c r="B99" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C99" s="6"/>
       <c r="D99">
         <v>0.5</v>
       </c>
-      <c r="E99" s="2"/>
+      <c r="E99" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
+      <c r="H99" s="2" t="s">
+        <v>212</v>
+      </c>
       <c r="I99" s="2"/>
       <c r="J99" s="6"/>
       <c r="K99">
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -2984,21 +3540,25 @@
       <c r="L100" s="9"/>
       <c r="M100" s="9"/>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C101" s="11"/>
       <c r="D101">
         <v>0.5</v>
       </c>
-      <c r="E101" s="10"/>
+      <c r="E101" s="10" t="s">
+        <v>167</v>
+      </c>
       <c r="F101" s="10"/>
       <c r="G101" s="10"/>
-      <c r="H101" s="10"/>
+      <c r="H101" s="10" t="s">
+        <v>213</v>
+      </c>
       <c r="I101" s="10"/>
       <c r="J101" s="11"/>
       <c r="K101" s="9">
@@ -3007,12 +3567,12 @@
       <c r="L101" s="9"/>
       <c r="M101" s="9"/>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C102"/>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C103" s="8">
         <f>SUM(C8:C101)</f>
@@ -3023,28 +3583,30 @@
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="C104"/>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C105"/>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C106" s="11"/>
       <c r="D106">
         <v>10</v>
       </c>
-      <c r="E106" s="10"/>
+      <c r="E106" s="10" t="s">
+        <v>168</v>
+      </c>
       <c r="F106" s="10"/>
       <c r="G106" s="10"/>
       <c r="H106" s="10"/>
@@ -3054,18 +3616,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C107" s="11"/>
       <c r="D107">
         <v>15</v>
       </c>
-      <c r="E107" s="10"/>
+      <c r="E107" s="10" t="s">
+        <v>169</v>
+      </c>
       <c r="F107" s="10"/>
       <c r="G107" s="10"/>
       <c r="H107" s="10"/>
@@ -3075,9 +3639,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="8">
@@ -3089,116 +3653,116 @@
         <v>125</v>
       </c>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C112" s="6"/>
       <c r="D112">
         <v>-10</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C113" s="6"/>
       <c r="D113">
         <v>-10</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C114" s="6"/>
       <c r="D114">
         <v>-25</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C115" s="6"/>
       <c r="D115">
         <v>-25</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C116" s="6"/>
       <c r="D116">
         <v>-25</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C117" s="6"/>
       <c r="D117">
         <v>-40</v>
       </c>
       <c r="E117" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C118" s="6"/>
       <c r="D118">
         <v>-50</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C119" s="6"/>
       <c r="D119">
         <v>-25</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C120" s="6"/>
       <c r="D120">
         <v>-25</v>
       </c>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C121" s="6"/>
       <c r="D121">
         <v>-80</v>
       </c>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C122" s="6"/>
       <c r="D122">
         <v>-50</v>
       </c>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C124" s="7">
         <f>C108-SUM(C112:C120)</f>

</xml_diff>

<commit_message>
misc: update tracibility table
</commit_message>
<xml_diff>
--- a/MaxwellMichael-grid.xlsx
+++ b/MaxwellMichael-grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PROLE\Documents\GitHub\poker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F66AA71-683E-4E96-83D7-0E3B09EB4E11}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C50ED25-D66E-41B7-9FB4-4867DAD61A1C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="213">
   <si>
     <t>You have coded your dependencies using Maven</t>
   </si>
@@ -480,9 +480,6 @@
   </si>
   <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>testRoyalFlush</t>
@@ -1709,8 +1706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I120" sqref="I120"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1836,7 +1833,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11">
@@ -1848,7 +1845,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12">
@@ -1870,7 +1867,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1891,7 +1888,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -1912,7 +1909,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1933,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1954,7 +1951,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1975,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1996,7 +1993,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -2017,7 +2014,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -2038,7 +2035,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -2059,7 +2056,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -2086,7 +2083,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -2113,7 +2110,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -2134,7 +2131,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -2155,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -2176,7 +2173,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -2197,7 +2194,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -2218,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -2239,7 +2236,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -2260,7 +2257,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -2281,7 +2278,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -2390,12 +2387,12 @@
         <v>0.5</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="6"/>
@@ -2415,12 +2412,12 @@
         <v>0.5</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="6"/>
@@ -2440,12 +2437,12 @@
         <v>0.5</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="6"/>
@@ -2465,12 +2462,12 @@
         <v>0.5</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="6"/>
@@ -2490,12 +2487,12 @@
         <v>0.5</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="6"/>
@@ -2515,12 +2512,12 @@
         <v>0.5</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="6"/>
@@ -2540,12 +2537,12 @@
         <v>0.5</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="6"/>
@@ -2565,12 +2562,12 @@
         <v>0.5</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="6"/>
@@ -2590,12 +2587,12 @@
         <v>0.5</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="6"/>
@@ -2615,12 +2612,12 @@
         <v>0.5</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="6"/>
@@ -2640,12 +2637,12 @@
         <v>0.5</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="6"/>
@@ -2665,12 +2662,12 @@
         <v>0.5</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="6"/>
@@ -2690,12 +2687,12 @@
         <v>0.5</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="6"/>
@@ -2715,12 +2712,12 @@
         <v>0.5</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="6"/>
@@ -2740,12 +2737,12 @@
         <v>0.5</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="6"/>
@@ -2765,12 +2762,12 @@
         <v>0.5</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="6"/>
@@ -2799,12 +2796,12 @@
         <v>0.25</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="6"/>
@@ -2825,12 +2822,12 @@
         <v>0.5</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I64" s="2"/>
       <c r="J64" s="6"/>
@@ -2851,12 +2848,12 @@
         <v>0.25</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I65" s="2"/>
       <c r="J65" s="6"/>
@@ -2877,12 +2874,12 @@
         <v>0.25</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I66" s="2"/>
       <c r="J66" s="6"/>
@@ -2903,12 +2900,12 @@
         <v>0.25</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I67" s="2"/>
       <c r="J67" s="6"/>
@@ -2929,12 +2926,12 @@
         <v>0.25</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I68" s="2"/>
       <c r="J68" s="6"/>
@@ -2955,12 +2952,12 @@
         <v>0.25</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I69" s="2"/>
       <c r="J69" s="6"/>
@@ -2981,12 +2978,12 @@
         <v>0.25</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I70" s="2"/>
       <c r="J70" s="6"/>
@@ -3007,12 +3004,12 @@
         <v>0.25</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I71" s="2"/>
       <c r="J71" s="6"/>
@@ -3048,12 +3045,12 @@
         <v>0.5</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I75" s="2"/>
       <c r="J75" s="6"/>
@@ -3073,12 +3070,12 @@
         <v>0.5</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I76" s="2"/>
       <c r="J76" s="6"/>
@@ -3098,12 +3095,12 @@
         <v>0.5</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I77" s="2"/>
       <c r="J77" s="6"/>
@@ -3123,12 +3120,12 @@
         <v>0.5</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I78" s="2"/>
       <c r="J78" s="6"/>
@@ -3148,12 +3145,12 @@
         <v>0.5</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I79" s="2"/>
       <c r="J79" s="6"/>
@@ -3173,12 +3170,12 @@
         <v>0.5</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I80" s="2"/>
       <c r="J80" s="6"/>
@@ -3204,12 +3201,12 @@
         <v>0.5</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I82" s="2"/>
       <c r="J82" s="6"/>
@@ -3229,12 +3226,12 @@
         <v>0.5</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I83" s="2"/>
       <c r="J83" s="6"/>
@@ -3266,12 +3263,12 @@
         <v>0.5</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I85" s="2"/>
       <c r="J85" s="6"/>
@@ -3291,12 +3288,12 @@
         <v>0.5</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I86" s="2"/>
       <c r="J86" s="6"/>
@@ -3312,12 +3309,12 @@
         <v>127</v>
       </c>
       <c r="E87" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F87" s="17"/>
       <c r="G87" s="17"/>
       <c r="H87" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I87" s="17"/>
       <c r="J87" s="18"/>
@@ -3340,12 +3337,12 @@
         <v>0.5</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I89" s="2"/>
       <c r="J89" s="6"/>
@@ -3370,12 +3367,12 @@
         <v>0.5</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I91" s="2"/>
       <c r="J91" s="6"/>
@@ -3400,12 +3397,12 @@
         <v>0.5</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I93" s="2"/>
       <c r="J93" s="6"/>
@@ -3425,12 +3422,12 @@
         <v>0.5</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I94" s="2"/>
       <c r="J94" s="6"/>
@@ -3450,12 +3447,12 @@
         <v>0.5</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I95" s="2"/>
       <c r="J95" s="6"/>
@@ -3480,12 +3477,12 @@
         <v>0.5</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I97" s="2"/>
       <c r="J97" s="6"/>
@@ -3510,12 +3507,12 @@
         <v>0.5</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I99" s="2"/>
       <c r="J99" s="6"/>
@@ -3552,12 +3549,12 @@
         <v>0.5</v>
       </c>
       <c r="E101" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F101" s="10"/>
       <c r="G101" s="10"/>
       <c r="H101" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I101" s="10"/>
       <c r="J101" s="11"/>
@@ -3605,7 +3602,7 @@
         <v>10</v>
       </c>
       <c r="E106" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F106" s="10"/>
       <c r="G106" s="10"/>
@@ -3628,7 +3625,7 @@
         <v>15</v>
       </c>
       <c r="E107" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F107" s="10"/>
       <c r="G107" s="10"/>

</xml_diff>